<commit_message>
updated ramadan dates with festive holiday dates
</commit_message>
<xml_diff>
--- a/ramadan_dates.xlsx
+++ b/ramadan_dates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\Desktop\R portfolio\PSET3\Final-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8210C1-D4A3-406E-9514-C349C06EE43D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3B1588-9D56-4D5C-BD5F-FC5D93135546}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="12473" xr2:uid="{4739C26E-F9DB-4F42-A458-4A4707837E21}"/>
   </bookViews>
@@ -31,22 +31,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="7">
   <si>
-    <t>Start</t>
+    <t>Holiday</t>
   </si>
   <si>
-    <t>End</t>
+    <t xml:space="preserve">Ramadan </t>
   </si>
   <si>
-    <t>Year</t>
+    <t>Eid al-Fitr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eid-al-adha </t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,6 +68,12 @@
     </font>
     <font>
       <sz val="5"/>
+      <color rgb="FF454545"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color rgb="FF454545"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -93,7 +111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -103,6 +121,7 @@
     <xf numFmtId="16" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA8BC071-9F8A-4E9D-A98C-A35DFF28314D}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -428,18 +447,21 @@
     <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>2004</v>
       </c>
@@ -447,11 +469,14 @@
         <v>38276</v>
       </c>
       <c r="C2" s="1">
-        <f xml:space="preserve"> B2 + 30</f>
-        <v>38306</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+        <f xml:space="preserve"> B2 + 29</f>
+        <v>38305</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2005</v>
       </c>
@@ -462,8 +487,11 @@
         <f xml:space="preserve"> B3 + 30</f>
         <v>38660</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2006</v>
       </c>
@@ -474,8 +502,11 @@
         <f t="shared" ref="C4:C16" si="0" xml:space="preserve"> B4 + 30</f>
         <v>39014</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>2007</v>
       </c>
@@ -486,8 +517,11 @@
         <f t="shared" si="0"/>
         <v>39368</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>2008</v>
       </c>
@@ -498,8 +532,11 @@
         <f t="shared" si="0"/>
         <v>39723</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>2009</v>
       </c>
@@ -510,8 +547,11 @@
         <f t="shared" si="0"/>
         <v>40077</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>2010</v>
       </c>
@@ -522,8 +562,11 @@
         <f t="shared" si="0"/>
         <v>40431</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>2011</v>
       </c>
@@ -534,8 +577,11 @@
         <f t="shared" si="0"/>
         <v>40786</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>2012</v>
       </c>
@@ -546,8 +592,11 @@
         <f t="shared" si="0"/>
         <v>41140</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>2013</v>
       </c>
@@ -558,8 +607,11 @@
         <f t="shared" si="0"/>
         <v>41494</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>2014</v>
       </c>
@@ -570,8 +622,11 @@
         <f t="shared" si="0"/>
         <v>41849</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>2015</v>
       </c>
@@ -582,8 +637,11 @@
         <f t="shared" si="0"/>
         <v>42203</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>2016</v>
       </c>
@@ -591,11 +649,14 @@
         <v>42528</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" si="0"/>
-        <v>42558</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+        <f xml:space="preserve"> B14 + 29</f>
+        <v>42557</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>2017</v>
       </c>
@@ -606,8 +667,11 @@
         <f t="shared" si="0"/>
         <v>42912</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>2018</v>
       </c>
@@ -617,6 +681,474 @@
       <c r="C16" s="1">
         <f t="shared" si="0"/>
         <v>43266</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>2004</v>
+      </c>
+      <c r="B17" s="1">
+        <f>$C$2</f>
+        <v>38305</v>
+      </c>
+      <c r="C17" s="1">
+        <f>B17 + 2</f>
+        <v>38307</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>2005</v>
+      </c>
+      <c r="B18" s="1">
+        <f t="shared" ref="B18:B31" si="1">C3</f>
+        <v>38660</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" ref="C18:C31" si="2">B18 + 2</f>
+        <v>38662</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>2006</v>
+      </c>
+      <c r="B19" s="1">
+        <f t="shared" si="1"/>
+        <v>39014</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="2"/>
+        <v>39016</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>2007</v>
+      </c>
+      <c r="B20" s="1">
+        <f t="shared" si="1"/>
+        <v>39368</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="2"/>
+        <v>39370</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>2008</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" si="1"/>
+        <v>39723</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="2"/>
+        <v>39725</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>2009</v>
+      </c>
+      <c r="B22" s="1">
+        <f t="shared" si="1"/>
+        <v>40077</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="2"/>
+        <v>40079</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>2010</v>
+      </c>
+      <c r="B23" s="1">
+        <f t="shared" si="1"/>
+        <v>40431</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="2"/>
+        <v>40433</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>2011</v>
+      </c>
+      <c r="B24" s="1">
+        <f t="shared" si="1"/>
+        <v>40786</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" si="2"/>
+        <v>40788</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>2012</v>
+      </c>
+      <c r="B25" s="1">
+        <f t="shared" si="1"/>
+        <v>41140</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" si="2"/>
+        <v>41142</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>2013</v>
+      </c>
+      <c r="B26" s="1">
+        <f t="shared" si="1"/>
+        <v>41494</v>
+      </c>
+      <c r="C26" s="1">
+        <f t="shared" si="2"/>
+        <v>41496</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>2014</v>
+      </c>
+      <c r="B27" s="1">
+        <f t="shared" si="1"/>
+        <v>41849</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" si="2"/>
+        <v>41851</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>2015</v>
+      </c>
+      <c r="B28" s="1">
+        <f t="shared" si="1"/>
+        <v>42203</v>
+      </c>
+      <c r="C28" s="1">
+        <f t="shared" si="2"/>
+        <v>42205</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>2016</v>
+      </c>
+      <c r="B29" s="1">
+        <f t="shared" si="1"/>
+        <v>42557</v>
+      </c>
+      <c r="C29" s="1">
+        <f t="shared" si="2"/>
+        <v>42559</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>2017</v>
+      </c>
+      <c r="B30" s="1">
+        <f t="shared" si="1"/>
+        <v>42912</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" si="2"/>
+        <v>42914</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>2018</v>
+      </c>
+      <c r="B31" s="1">
+        <f t="shared" si="1"/>
+        <v>43266</v>
+      </c>
+      <c r="C31" s="1">
+        <f t="shared" si="2"/>
+        <v>43268</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>2004</v>
+      </c>
+      <c r="B32" s="1">
+        <v>38018</v>
+      </c>
+      <c r="C32" s="1">
+        <f xml:space="preserve"> B32 + 1</f>
+        <v>38019</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>2005</v>
+      </c>
+      <c r="B33" s="1">
+        <v>38372</v>
+      </c>
+      <c r="C33" s="1">
+        <f t="shared" ref="C33:C46" si="3" xml:space="preserve"> B33 + 1</f>
+        <v>38373</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>2006</v>
+      </c>
+      <c r="B34" s="1">
+        <v>39081</v>
+      </c>
+      <c r="C34" s="1">
+        <f t="shared" si="3"/>
+        <v>39082</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>2007</v>
+      </c>
+      <c r="B35" s="1">
+        <v>39434</v>
+      </c>
+      <c r="C35" s="1">
+        <f t="shared" si="3"/>
+        <v>39435</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>2008</v>
+      </c>
+      <c r="B36" s="1">
+        <v>39790</v>
+      </c>
+      <c r="C36" s="1">
+        <f t="shared" si="3"/>
+        <v>39791</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>2009</v>
+      </c>
+      <c r="B37" s="1">
+        <v>40143</v>
+      </c>
+      <c r="C37" s="1">
+        <f t="shared" si="3"/>
+        <v>40144</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>2010</v>
+      </c>
+      <c r="B38" s="1">
+        <v>40497</v>
+      </c>
+      <c r="C38" s="1">
+        <f t="shared" si="3"/>
+        <v>40498</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>2011</v>
+      </c>
+      <c r="B39" s="1">
+        <v>40852</v>
+      </c>
+      <c r="C39" s="1">
+        <f t="shared" si="3"/>
+        <v>40853</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>2012</v>
+      </c>
+      <c r="B40" s="1">
+        <v>41207</v>
+      </c>
+      <c r="C40" s="1">
+        <f t="shared" si="3"/>
+        <v>41208</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>2013</v>
+      </c>
+      <c r="B41" s="2">
+        <v>41562</v>
+      </c>
+      <c r="C41" s="1">
+        <f t="shared" si="3"/>
+        <v>41563</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>2014</v>
+      </c>
+      <c r="B42" s="2">
+        <v>41917</v>
+      </c>
+      <c r="C42" s="1">
+        <f t="shared" si="3"/>
+        <v>41918</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>2015</v>
+      </c>
+      <c r="B43" s="4">
+        <v>42271</v>
+      </c>
+      <c r="C43" s="1">
+        <f t="shared" si="3"/>
+        <v>42272</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>2016</v>
+      </c>
+      <c r="B44" s="3">
+        <v>42626</v>
+      </c>
+      <c r="C44" s="1">
+        <f t="shared" si="3"/>
+        <v>42627</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>2017</v>
+      </c>
+      <c r="B45" s="3">
+        <v>42980</v>
+      </c>
+      <c r="C45" s="1">
+        <f t="shared" si="3"/>
+        <v>42981</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>2018</v>
+      </c>
+      <c r="B46" s="3">
+        <v>43334</v>
+      </c>
+      <c r="C46" s="1">
+        <f t="shared" si="3"/>
+        <v>43335</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commiting improved holiday code
</commit_message>
<xml_diff>
--- a/ramadan_dates.xlsx
+++ b/ramadan_dates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\Desktop\R portfolio\PSET3\Final-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3B1588-9D56-4D5C-BD5F-FC5D93135546}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3538A3E2-4192-4DCF-8924-52E8EC5D348F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="12473" xr2:uid="{4739C26E-F9DB-4F42-A458-4A4707837E21}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="9">
   <si>
     <t>Holiday</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Celebratory </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FALSE </t>
   </si>
 </sst>
 </file>
@@ -436,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA8BC071-9F8A-4E9D-A98C-A35DFF28314D}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -447,7 +453,7 @@
     <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -460,8 +466,11 @@
       <c r="D1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>2004</v>
       </c>
@@ -475,8 +484,11 @@
       <c r="D2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2005</v>
       </c>
@@ -490,8 +502,11 @@
       <c r="D3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2006</v>
       </c>
@@ -505,8 +520,11 @@
       <c r="D4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>2007</v>
       </c>
@@ -520,8 +538,11 @@
       <c r="D5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>2008</v>
       </c>
@@ -535,8 +556,11 @@
       <c r="D6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>2009</v>
       </c>
@@ -550,8 +574,11 @@
       <c r="D7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>2010</v>
       </c>
@@ -565,8 +592,11 @@
       <c r="D8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>2011</v>
       </c>
@@ -580,8 +610,11 @@
       <c r="D9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>2012</v>
       </c>
@@ -595,8 +628,11 @@
       <c r="D10" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>2013</v>
       </c>
@@ -610,8 +646,11 @@
       <c r="D11" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>2014</v>
       </c>
@@ -625,8 +664,11 @@
       <c r="D12" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>2015</v>
       </c>
@@ -640,8 +682,11 @@
       <c r="D13" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>2016</v>
       </c>
@@ -655,8 +700,11 @@
       <c r="D14" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>2017</v>
       </c>
@@ -670,8 +718,11 @@
       <c r="D15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>2018</v>
       </c>
@@ -685,8 +736,11 @@
       <c r="D16" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>2004</v>
       </c>
@@ -701,8 +755,11 @@
       <c r="D17" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>2005</v>
       </c>
@@ -717,8 +774,11 @@
       <c r="D18" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>2006</v>
       </c>
@@ -733,8 +793,11 @@
       <c r="D19" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>2007</v>
       </c>
@@ -749,8 +812,11 @@
       <c r="D20" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>2008</v>
       </c>
@@ -765,8 +831,11 @@
       <c r="D21" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>2009</v>
       </c>
@@ -781,8 +850,11 @@
       <c r="D22" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>2010</v>
       </c>
@@ -797,8 +869,11 @@
       <c r="D23" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>2011</v>
       </c>
@@ -813,8 +888,11 @@
       <c r="D24" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>2012</v>
       </c>
@@ -829,8 +907,11 @@
       <c r="D25" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>2013</v>
       </c>
@@ -845,8 +926,11 @@
       <c r="D26" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>2014</v>
       </c>
@@ -861,8 +945,11 @@
       <c r="D27" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>2015</v>
       </c>
@@ -877,8 +964,11 @@
       <c r="D28" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>2016</v>
       </c>
@@ -893,8 +983,11 @@
       <c r="D29" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>2017</v>
       </c>
@@ -909,8 +1002,11 @@
       <c r="D30" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>2018</v>
       </c>
@@ -925,8 +1021,11 @@
       <c r="D31" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>2004</v>
       </c>
@@ -940,8 +1039,11 @@
       <c r="D32" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>2005</v>
       </c>
@@ -955,8 +1057,11 @@
       <c r="D33" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>2006</v>
       </c>
@@ -970,8 +1075,11 @@
       <c r="D34" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>2007</v>
       </c>
@@ -985,8 +1093,11 @@
       <c r="D35" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>2008</v>
       </c>
@@ -1000,8 +1111,11 @@
       <c r="D36" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>2009</v>
       </c>
@@ -1015,8 +1129,11 @@
       <c r="D37" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>2010</v>
       </c>
@@ -1030,8 +1147,11 @@
       <c r="D38" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>2011</v>
       </c>
@@ -1045,8 +1165,11 @@
       <c r="D39" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>2012</v>
       </c>
@@ -1060,8 +1183,11 @@
       <c r="D40" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>2013</v>
       </c>
@@ -1075,8 +1201,11 @@
       <c r="D41" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>2014</v>
       </c>
@@ -1090,8 +1219,11 @@
       <c r="D42" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>2015</v>
       </c>
@@ -1105,8 +1237,11 @@
       <c r="D43" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>2016</v>
       </c>
@@ -1120,8 +1255,11 @@
       <c r="D44" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>2017</v>
       </c>
@@ -1135,8 +1273,11 @@
       <c r="D45" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>2018</v>
       </c>
@@ -1149,6 +1290,9 @@
       </c>
       <c r="D46" s="5" t="s">
         <v>3</v>
+      </c>
+      <c r="E46" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>